<commit_message>
Esercizi settimanali svolti Modulo 1
</commit_message>
<xml_diff>
--- a/ESERCIZIO_M2-1-1 Risolto. Marco Sanna.xlsx
+++ b/ESERCIZIO_M2-1-1 Risolto. Marco Sanna.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/336bfa5fe63ea8b3/Desktop/Esercizi Data Analyst/Esercizi Svolti/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{E47AFB31-6233-4FC1-8755-62937E8444BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E77801EC-B098-4F56-8303-E5AD1B81F7F5}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{E47AFB31-6233-4FC1-8755-62937E8444BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0965E6ED-2D84-4C77-92EA-10C41F2F6D28}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="216" windowWidth="11604" windowHeight="12036" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="924" windowWidth="11604" windowHeight="12036" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assoluti_Iva" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2259,6 +2259,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:G8" headerRowCount="0">
   <tableColumns count="7">
@@ -34325,8 +34329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -62255,19 +62259,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="24" width="8.6640625" customWidth="1"/>
@@ -62463,7 +62467,7 @@
         <v>501</v>
       </c>
       <c r="H7" s="16">
-        <f t="shared" ref="H7:H13" si="1">COUNTIF(B2:B85,G7)</f>
+        <f>COUNTIF($B$2:$B$85,G7)</f>
         <v>2</v>
       </c>
       <c r="I7" s="17">
@@ -62492,7 +62496,7 @@
         <v>507</v>
       </c>
       <c r="H8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H8:H13" si="1">COUNTIF($B$2:$B$85,G8)</f>
         <v>1</v>
       </c>
       <c r="I8" s="17">

</xml_diff>